<commit_message>
Hotfix: Remise sprint 2
</commit_message>
<xml_diff>
--- a/Equipe302.xlsx
+++ b/Equipe302.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="601" documentId="8_{A9B08717-0A78-4896-A8AA-F48CA0C7A758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53A0E9C2-6B32-4E64-9930-F0255D8A0CC8}"/>
+  <xr:revisionPtr revIDLastSave="611" documentId="8_{A9B08717-0A78-4896-A8AA-F48CA0C7A758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88F76A75-A0C9-4095-A009-D0BD1349191A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="9" r:id="rId1"/>
@@ -1769,9 +1769,6 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2492,6 +2489,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2899,115 +2899,115 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="30">
-      <c r="A3" s="41"/>
-      <c r="B3" s="127" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="127" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="127" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="126" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="128" t="s">
+      <c r="E3" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="129" t="s">
+      <c r="F3" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="130" t="s">
+      <c r="G3" s="129" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="109">
+      <c r="B4" s="108">
         <f>(Fonctionnalités!E18)</f>
         <v>0.82254545454545447</v>
       </c>
-      <c r="C4" s="109">
+      <c r="C4" s="108">
         <f>'Assurance Qualité'!C60</f>
         <v>0.73466666666666669</v>
       </c>
-      <c r="D4" s="109">
+      <c r="D4" s="108">
         <f>B4*0.6+C4*0.4 - 0.1*E4</f>
         <v>0.78739393939393931</v>
       </c>
-      <c r="E4" s="110"/>
-      <c r="F4" s="111">
+      <c r="E4" s="109"/>
+      <c r="F4" s="110">
         <v>20</v>
       </c>
-      <c r="G4" s="112">
+      <c r="G4" s="111">
         <f>D4*F4</f>
         <v>15.747878787878786</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="114">
+      <c r="B5" s="113">
         <f>(Fonctionnalités!E34)</f>
         <v>0.83102962962962967</v>
       </c>
-      <c r="C5" s="114">
+      <c r="C5" s="113">
         <f>'Assurance Qualité'!F60</f>
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="D5" s="114">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="D5" s="113">
         <f t="shared" ref="D5:D6" si="0">B5*0.6+C5*0.4 - 0.1*E5</f>
-        <v>0.76861777777777784</v>
-      </c>
-      <c r="E5" s="115"/>
-      <c r="F5" s="116">
+        <v>0.77341777777777776</v>
+      </c>
+      <c r="E5" s="114"/>
+      <c r="F5" s="115">
         <v>25</v>
       </c>
-      <c r="G5" s="117">
+      <c r="G5" s="116">
         <f t="shared" ref="G5:G7" si="1">D5*F5</f>
-        <v>19.215444444444447</v>
+        <v>19.335444444444445</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="119">
+      <c r="B6" s="118">
         <f>(Fonctionnalités!E50)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="119">
+      <c r="C6" s="118">
         <f>'Assurance Qualité'!I60</f>
         <v>0</v>
       </c>
-      <c r="D6" s="119">
+      <c r="D6" s="118">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="120"/>
-      <c r="F6" s="121">
+      <c r="E6" s="119"/>
+      <c r="F6" s="120">
         <v>20</v>
       </c>
-      <c r="G6" s="122">
+      <c r="G6" s="121">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="123" t="s">
+      <c r="A7" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="123"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="124">
-        <v>0</v>
-      </c>
-      <c r="E7" s="125"/>
-      <c r="F7" s="123">
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="123">
+        <v>0</v>
+      </c>
+      <c r="E7" s="124"/>
+      <c r="F7" s="122">
         <v>10</v>
       </c>
-      <c r="G7" s="126">
+      <c r="G7" s="125">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3022,1069 +3022,1069 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" style="38" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="38"/>
-    <col min="4" max="4" width="9.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="38" customWidth="1"/>
-    <col min="7" max="7" width="54.85546875" style="38" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="38"/>
+    <col min="1" max="1" width="50.5703125" style="37" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="37"/>
+    <col min="4" max="4" width="9.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="37" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" style="37" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="37"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="229" t="s">
+      <c r="A2" s="228" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="229"/>
-      <c r="C2" s="229"/>
-      <c r="D2" s="229"/>
-      <c r="E2" s="229"/>
-      <c r="F2" s="229"/>
-      <c r="G2" s="229"/>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7" ht="18.75">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:7" ht="23.25">
-      <c r="A6" s="233" t="s">
+      <c r="A6" s="232" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="234"/>
-      <c r="C6" s="234"/>
-      <c r="D6" s="234"/>
-      <c r="E6" s="234"/>
-      <c r="F6" s="234"/>
-      <c r="G6" s="235"/>
+      <c r="B6" s="233"/>
+      <c r="C6" s="233"/>
+      <c r="D6" s="233"/>
+      <c r="E6" s="233"/>
+      <c r="F6" s="233"/>
+      <c r="G6" s="234"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="131" t="s">
+      <c r="A7" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="132" t="s">
+      <c r="B7" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="131" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="E7" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="F7" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="133" t="s">
+      <c r="G7" s="132" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="134" t="s">
+      <c r="A8" s="133" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="135">
-        <v>1</v>
-      </c>
-      <c r="C8" s="135">
-        <v>1</v>
-      </c>
-      <c r="D8" s="135">
+      <c r="B8" s="134">
+        <v>1</v>
+      </c>
+      <c r="C8" s="134">
+        <v>1</v>
+      </c>
+      <c r="D8" s="134">
         <v>4</v>
       </c>
-      <c r="E8" s="135">
+      <c r="E8" s="134">
         <f t="shared" ref="E8:E17" si="0">B8*C8*D8</f>
         <v>4</v>
       </c>
-      <c r="F8" s="135" t="s">
+      <c r="F8" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="136"/>
+      <c r="G8" s="135"/>
     </row>
     <row r="9" spans="1:7" ht="60">
-      <c r="A9" s="137" t="s">
+      <c r="A9" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="138">
+      <c r="B9" s="137">
         <f>10/11</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="C9" s="138">
+      <c r="C9" s="137">
         <v>0.75</v>
       </c>
-      <c r="D9" s="138">
+      <c r="D9" s="137">
         <v>8</v>
       </c>
-      <c r="E9" s="138">
+      <c r="E9" s="137">
         <f t="shared" si="0"/>
         <v>5.4545454545454541</v>
       </c>
-      <c r="F9" s="138" t="s">
+      <c r="F9" s="137" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="220" t="s">
+      <c r="G9" s="219" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="120">
-      <c r="A10" s="134" t="s">
+      <c r="A10" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="135">
+      <c r="B10" s="134">
         <f>23/25</f>
         <v>0.92</v>
       </c>
-      <c r="C10" s="135">
+      <c r="C10" s="134">
         <v>0.75</v>
       </c>
-      <c r="D10" s="135">
+      <c r="D10" s="134">
         <v>20</v>
       </c>
-      <c r="E10" s="135">
+      <c r="E10" s="134">
         <f t="shared" si="0"/>
         <v>13.8</v>
       </c>
-      <c r="F10" s="135" t="s">
+      <c r="F10" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="221" t="s">
+      <c r="G10" s="220" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30.75">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="138">
+      <c r="B11" s="137">
         <f>(9/10)</f>
         <v>0.9</v>
       </c>
-      <c r="C11" s="138">
-        <v>1</v>
-      </c>
-      <c r="D11" s="138">
+      <c r="C11" s="137">
+        <v>1</v>
+      </c>
+      <c r="D11" s="137">
         <v>10</v>
       </c>
-      <c r="E11" s="138">
+      <c r="E11" s="137">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F11" s="138" t="s">
+      <c r="F11" s="137" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="220" t="s">
+      <c r="G11" s="219" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="134" t="s">
+      <c r="A12" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="135">
-        <v>1</v>
-      </c>
-      <c r="C12" s="135">
-        <v>1</v>
-      </c>
-      <c r="D12" s="135">
+      <c r="B12" s="134">
+        <v>1</v>
+      </c>
+      <c r="C12" s="134">
+        <v>1</v>
+      </c>
+      <c r="D12" s="134">
         <v>10</v>
       </c>
-      <c r="E12" s="135">
+      <c r="E12" s="134">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F12" s="135" t="s">
+      <c r="F12" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="136"/>
+      <c r="G12" s="135"/>
     </row>
     <row r="13" spans="1:7" ht="60.75">
-      <c r="A13" s="134" t="s">
+      <c r="A13" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="135">
+      <c r="B13" s="134">
         <f>(11/12)</f>
         <v>0.91666666666666663</v>
       </c>
-      <c r="C13" s="135">
-        <v>1</v>
-      </c>
-      <c r="D13" s="135">
+      <c r="C13" s="134">
+        <v>1</v>
+      </c>
+      <c r="D13" s="134">
         <v>12</v>
       </c>
-      <c r="E13" s="135">
+      <c r="E13" s="134">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="F13" s="135" t="s">
+      <c r="F13" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="221" t="s">
+      <c r="G13" s="220" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="137" t="s">
+      <c r="A14" s="136" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="138">
+      <c r="B14" s="137">
         <f>11/12</f>
         <v>0.91666666666666663</v>
       </c>
-      <c r="C14" s="138">
-        <v>1</v>
-      </c>
-      <c r="D14" s="138">
+      <c r="C14" s="137">
+        <v>1</v>
+      </c>
+      <c r="D14" s="137">
         <v>12</v>
       </c>
-      <c r="E14" s="138">
+      <c r="E14" s="137">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="F14" s="138" t="s">
+      <c r="F14" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="139" t="s">
+      <c r="G14" s="138" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="134" t="s">
+      <c r="A15" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="135">
-        <v>1</v>
-      </c>
-      <c r="C15" s="135">
-        <v>1</v>
-      </c>
-      <c r="D15" s="135">
+      <c r="B15" s="134">
+        <v>1</v>
+      </c>
+      <c r="C15" s="134">
+        <v>1</v>
+      </c>
+      <c r="D15" s="134">
         <v>10</v>
       </c>
-      <c r="E15" s="135">
+      <c r="E15" s="134">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F15" s="135" t="s">
+      <c r="F15" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="136"/>
+      <c r="G15" s="135"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="137" t="s">
+      <c r="A16" s="136" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="138">
-        <v>1</v>
-      </c>
-      <c r="C16" s="138">
-        <v>1</v>
-      </c>
-      <c r="D16" s="138">
+      <c r="B16" s="137">
+        <v>1</v>
+      </c>
+      <c r="C16" s="137">
+        <v>1</v>
+      </c>
+      <c r="D16" s="137">
         <v>8</v>
       </c>
-      <c r="E16" s="138">
+      <c r="E16" s="137">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F16" s="138" t="s">
+      <c r="F16" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="139"/>
+      <c r="G16" s="138"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="140" t="s">
+      <c r="A17" s="139" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="141">
+      <c r="B17" s="140">
         <f>5/6</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="C17" s="141">
-        <v>1</v>
-      </c>
-      <c r="D17" s="141">
+      <c r="C17" s="140">
+        <v>1</v>
+      </c>
+      <c r="D17" s="140">
         <v>6</v>
       </c>
-      <c r="E17" s="141">
+      <c r="E17" s="140">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F17" s="141" t="s">
+      <c r="F17" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="142" t="s">
+      <c r="G17" s="141" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="143" t="s">
+      <c r="A18" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="236"/>
-      <c r="C18" s="236"/>
-      <c r="D18" s="144">
+      <c r="B18" s="235"/>
+      <c r="C18" s="235"/>
+      <c r="D18" s="143">
         <f>SUM(D8:D17)</f>
         <v>100</v>
       </c>
-      <c r="E18" s="145">
+      <c r="E18" s="144">
         <f>(SUM(E8:E17)+E20+E21)/D18</f>
         <v>0.82254545454545447</v>
       </c>
-      <c r="F18" s="145"/>
-      <c r="G18" s="146"/>
+      <c r="F18" s="144"/>
+      <c r="G18" s="145"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="147" t="s">
+      <c r="A19" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="148" t="s">
+      <c r="B19" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="148"/>
-      <c r="D19" s="148" t="s">
+      <c r="C19" s="147"/>
+      <c r="D19" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="149" t="s">
+      <c r="E19" s="148" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="149"/>
-      <c r="G19" s="150" t="s">
+      <c r="F19" s="148"/>
+      <c r="G19" s="149" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="60">
-      <c r="A20" s="151" t="s">
+      <c r="A20" s="150" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="152">
+      <c r="B20" s="151">
         <v>0.5</v>
       </c>
-      <c r="C20" s="152"/>
-      <c r="D20" s="153">
+      <c r="C20" s="151"/>
+      <c r="D20" s="152">
         <v>-10</v>
       </c>
-      <c r="E20" s="152">
+      <c r="E20" s="151">
         <f>B20*D20</f>
         <v>-5</v>
       </c>
-      <c r="F20" s="152"/>
-      <c r="G20" s="222" t="s">
+      <c r="F20" s="151"/>
+      <c r="G20" s="221" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="154" t="s">
+      <c r="A21" s="153" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="155">
-        <v>0</v>
-      </c>
-      <c r="C21" s="155"/>
-      <c r="D21" s="156">
+      <c r="B21" s="154">
+        <v>0</v>
+      </c>
+      <c r="C21" s="154"/>
+      <c r="D21" s="155">
         <v>-15</v>
       </c>
-      <c r="E21" s="155">
+      <c r="E21" s="154">
         <f>B21*D21</f>
         <v>0</v>
       </c>
-      <c r="F21" s="155"/>
-      <c r="G21" s="157"/>
+      <c r="F21" s="154"/>
+      <c r="G21" s="156"/>
     </row>
     <row r="22" spans="1:7" ht="23.25">
-      <c r="A22" s="237" t="s">
+      <c r="A22" s="236" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="238"/>
-      <c r="C22" s="238"/>
-      <c r="D22" s="238"/>
-      <c r="E22" s="238"/>
-      <c r="F22" s="238"/>
-      <c r="G22" s="239"/>
+      <c r="B22" s="237"/>
+      <c r="C22" s="237"/>
+      <c r="D22" s="237"/>
+      <c r="E22" s="237"/>
+      <c r="F22" s="237"/>
+      <c r="G22" s="238"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="158" t="s">
+      <c r="A23" s="157" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="159" t="s">
+      <c r="B23" s="158" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="159" t="s">
+      <c r="C23" s="158" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="159" t="s">
+      <c r="D23" s="158" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="159" t="s">
+      <c r="E23" s="158" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="159" t="s">
+      <c r="F23" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="160" t="s">
+      <c r="G23" s="159" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="137.25">
-      <c r="A24" s="161" t="s">
+      <c r="A24" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="162">
+      <c r="B24" s="161">
         <f>16/20</f>
         <v>0.8</v>
       </c>
-      <c r="C24" s="162">
-        <v>1</v>
-      </c>
-      <c r="D24" s="162">
+      <c r="C24" s="161">
+        <v>1</v>
+      </c>
+      <c r="D24" s="161">
         <v>20</v>
       </c>
-      <c r="E24" s="162">
+      <c r="E24" s="161">
         <f>B24*C24*D24</f>
         <v>16</v>
       </c>
-      <c r="F24" s="162" t="s">
+      <c r="F24" s="161" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="225" t="s">
+      <c r="G24" s="224" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="164" t="s">
+      <c r="A25" s="163" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="165">
-        <v>1</v>
-      </c>
-      <c r="C25" s="165">
-        <v>1</v>
-      </c>
-      <c r="D25" s="165">
+      <c r="B25" s="164">
+        <v>1</v>
+      </c>
+      <c r="C25" s="164">
+        <v>1</v>
+      </c>
+      <c r="D25" s="164">
         <v>6</v>
       </c>
-      <c r="E25" s="165">
+      <c r="E25" s="164">
         <f t="shared" ref="E25:E33" si="1">B25*C25*D25</f>
         <v>6</v>
       </c>
-      <c r="F25" s="165" t="s">
+      <c r="F25" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="166" t="s">
+      <c r="G25" s="165" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="106.5">
-      <c r="A26" s="161" t="s">
+      <c r="A26" s="160" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="162">
+      <c r="B26" s="161">
         <f>8/12</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C26" s="162">
-        <v>1</v>
-      </c>
-      <c r="D26" s="162">
+      <c r="C26" s="161">
+        <v>1</v>
+      </c>
+      <c r="D26" s="161">
         <v>12</v>
       </c>
-      <c r="E26" s="162">
+      <c r="E26" s="161">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F26" s="162" t="s">
+      <c r="F26" s="161" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="225" t="s">
+      <c r="G26" s="224" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="164" t="s">
+      <c r="A27" s="163" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="165">
-        <v>1</v>
-      </c>
-      <c r="C27" s="165">
-        <v>1</v>
-      </c>
-      <c r="D27" s="165">
+      <c r="B27" s="164">
+        <v>1</v>
+      </c>
+      <c r="C27" s="164">
+        <v>1</v>
+      </c>
+      <c r="D27" s="164">
         <v>8</v>
       </c>
-      <c r="E27" s="165">
+      <c r="E27" s="164">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F27" s="165" t="s">
+      <c r="F27" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="166" t="s">
+      <c r="G27" s="165" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30.75">
-      <c r="A28" s="161" t="s">
+      <c r="A28" s="160" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="162">
-        <v>1</v>
-      </c>
-      <c r="C28" s="162">
-        <v>1</v>
-      </c>
-      <c r="D28" s="162">
+      <c r="B28" s="161">
+        <v>1</v>
+      </c>
+      <c r="C28" s="161">
+        <v>1</v>
+      </c>
+      <c r="D28" s="161">
         <v>6</v>
       </c>
-      <c r="E28" s="162">
+      <c r="E28" s="161">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F28" s="162" t="s">
+      <c r="F28" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="228" t="s">
+      <c r="G28" s="227" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="60.75">
-      <c r="A29" s="164" t="s">
+      <c r="A29" s="163" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="165">
+      <c r="B29" s="164">
         <f>25/27</f>
         <v>0.92592592592592593</v>
       </c>
-      <c r="C29" s="165">
-        <v>1</v>
-      </c>
-      <c r="D29" s="165">
+      <c r="C29" s="164">
+        <v>1</v>
+      </c>
+      <c r="D29" s="164">
         <v>14</v>
       </c>
-      <c r="E29" s="165">
+      <c r="E29" s="164">
         <f t="shared" si="1"/>
         <v>12.962962962962964</v>
       </c>
-      <c r="F29" s="165" t="s">
+      <c r="F29" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="226" t="s">
+      <c r="G29" s="225" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="161" t="s">
+      <c r="A30" s="160" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="162">
-        <v>1</v>
-      </c>
-      <c r="C30" s="162">
-        <v>1</v>
-      </c>
-      <c r="D30" s="162">
+      <c r="B30" s="161">
+        <v>1</v>
+      </c>
+      <c r="C30" s="161">
+        <v>1</v>
+      </c>
+      <c r="D30" s="161">
         <v>12</v>
       </c>
-      <c r="E30" s="162">
+      <c r="E30" s="161">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="F30" s="162" t="s">
+      <c r="F30" s="161" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="163"/>
+      <c r="G30" s="162"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="164" t="s">
+      <c r="A31" s="163" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="165">
-        <v>1</v>
-      </c>
-      <c r="C31" s="165">
-        <v>1</v>
-      </c>
-      <c r="D31" s="165">
+      <c r="B31" s="164">
+        <v>1</v>
+      </c>
+      <c r="C31" s="164">
+        <v>1</v>
+      </c>
+      <c r="D31" s="164">
         <v>4</v>
       </c>
-      <c r="E31" s="165">
+      <c r="E31" s="164">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F31" s="165" t="s">
+      <c r="F31" s="164" t="s">
         <v>25</v>
       </c>
-      <c r="G31" s="226"/>
+      <c r="G31" s="225"/>
     </row>
     <row r="32" spans="1:7" ht="76.5">
-      <c r="A32" s="161" t="s">
+      <c r="A32" s="160" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="162">
+      <c r="B32" s="161">
         <f>14/16</f>
         <v>0.875</v>
       </c>
-      <c r="C32" s="162">
-        <v>1</v>
-      </c>
-      <c r="D32" s="162">
+      <c r="C32" s="161">
+        <v>1</v>
+      </c>
+      <c r="D32" s="161">
         <v>10</v>
       </c>
-      <c r="E32" s="162">
+      <c r="E32" s="161">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
-      <c r="F32" s="162" t="s">
+      <c r="F32" s="161" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="225" t="s">
+      <c r="G32" s="224" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="91.5">
-      <c r="A33" s="167" t="s">
+      <c r="A33" s="166" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="168">
+      <c r="B33" s="167">
         <v>0.33</v>
       </c>
-      <c r="C33" s="168">
-        <v>1</v>
-      </c>
-      <c r="D33" s="168">
+      <c r="C33" s="167">
+        <v>1</v>
+      </c>
+      <c r="D33" s="167">
         <v>8</v>
       </c>
-      <c r="E33" s="168">
+      <c r="E33" s="167">
         <f t="shared" si="1"/>
         <v>2.64</v>
       </c>
-      <c r="F33" s="168" t="s">
+      <c r="F33" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="227" t="s">
+      <c r="G33" s="226" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="169" t="s">
+      <c r="A34" s="168" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="170"/>
-      <c r="C34" s="170"/>
-      <c r="D34" s="170">
+      <c r="B34" s="169"/>
+      <c r="C34" s="169"/>
+      <c r="D34" s="169">
         <f>SUM(D24:D33)</f>
         <v>100</v>
       </c>
-      <c r="E34" s="171">
+      <c r="E34" s="170">
         <f>(SUM(E24:E33) + E36+E37+E38)/D34</f>
         <v>0.83102962962962967</v>
       </c>
-      <c r="F34" s="171"/>
-      <c r="G34" s="172"/>
+      <c r="F34" s="170"/>
+      <c r="G34" s="171"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="173" t="s">
+      <c r="A35" s="172" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="174" t="s">
+      <c r="B35" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="174"/>
-      <c r="D35" s="174" t="s">
+      <c r="C35" s="173"/>
+      <c r="D35" s="173" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="175" t="s">
+      <c r="E35" s="174" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="175"/>
-      <c r="G35" s="176" t="s">
+      <c r="F35" s="174"/>
+      <c r="G35" s="175" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="177" t="s">
+      <c r="A36" s="176" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="178">
-        <v>0</v>
-      </c>
-      <c r="C36" s="178"/>
-      <c r="D36" s="179">
+      <c r="B36" s="177">
+        <v>0</v>
+      </c>
+      <c r="C36" s="177"/>
+      <c r="D36" s="178">
         <v>-10</v>
       </c>
-      <c r="E36" s="178">
+      <c r="E36" s="177">
         <f>B36*D36</f>
         <v>0</v>
       </c>
-      <c r="F36" s="178"/>
-      <c r="G36" s="180"/>
+      <c r="F36" s="177"/>
+      <c r="G36" s="179"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="181" t="s">
+      <c r="A37" s="180" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="182">
-        <v>0</v>
-      </c>
-      <c r="C37" s="182"/>
-      <c r="D37" s="183">
+      <c r="B37" s="181">
+        <v>0</v>
+      </c>
+      <c r="C37" s="181"/>
+      <c r="D37" s="182">
         <v>-15</v>
       </c>
-      <c r="E37" s="182">
+      <c r="E37" s="181">
         <f>B37*D37</f>
         <v>0</v>
       </c>
-      <c r="F37" s="182"/>
-      <c r="G37" s="184"/>
+      <c r="F37" s="181"/>
+      <c r="G37" s="183"/>
     </row>
     <row r="38" spans="1:7" ht="45.75">
-      <c r="A38" s="185" t="s">
+      <c r="A38" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="186">
+      <c r="B38" s="185">
         <v>0.25</v>
       </c>
-      <c r="C38" s="186"/>
-      <c r="D38" s="187">
+      <c r="C38" s="185"/>
+      <c r="D38" s="186">
         <v>-5</v>
       </c>
-      <c r="E38" s="186">
+      <c r="E38" s="185">
         <f>B38*D38</f>
         <v>-1.25</v>
       </c>
-      <c r="F38" s="186"/>
-      <c r="G38" s="224" t="s">
+      <c r="F38" s="185"/>
+      <c r="G38" s="223" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="23.25">
-      <c r="A39" s="230" t="s">
+      <c r="A39" s="229" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="231"/>
-      <c r="C39" s="231"/>
-      <c r="D39" s="231"/>
-      <c r="E39" s="231"/>
-      <c r="F39" s="231"/>
-      <c r="G39" s="232"/>
+      <c r="B39" s="230"/>
+      <c r="C39" s="230"/>
+      <c r="D39" s="230"/>
+      <c r="E39" s="230"/>
+      <c r="F39" s="230"/>
+      <c r="G39" s="231"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="188" t="s">
+      <c r="A40" s="187" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="189" t="s">
+      <c r="B40" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="189" t="s">
+      <c r="C40" s="188" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="189" t="s">
+      <c r="D40" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="189" t="s">
+      <c r="E40" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="189" t="s">
+      <c r="F40" s="188" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="190" t="s">
+      <c r="G40" s="189" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="191" t="s">
+      <c r="A41" s="190" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="192">
-        <v>0</v>
-      </c>
-      <c r="C41" s="192">
-        <v>0</v>
-      </c>
-      <c r="D41" s="192">
+      <c r="B41" s="191">
+        <v>0</v>
+      </c>
+      <c r="C41" s="191">
+        <v>0</v>
+      </c>
+      <c r="D41" s="191">
         <v>16</v>
       </c>
-      <c r="E41" s="192">
+      <c r="E41" s="191">
         <f t="shared" ref="E41:E49" si="2">B41*C41*D41</f>
         <v>0</v>
       </c>
-      <c r="F41" s="192"/>
-      <c r="G41" s="193"/>
+      <c r="F41" s="191"/>
+      <c r="G41" s="192"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="194" t="s">
+      <c r="A42" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="195">
-        <v>0</v>
-      </c>
-      <c r="C42" s="195">
-        <v>0</v>
-      </c>
-      <c r="D42" s="195">
+      <c r="B42" s="194">
+        <v>0</v>
+      </c>
+      <c r="C42" s="194">
+        <v>0</v>
+      </c>
+      <c r="D42" s="194">
         <v>16</v>
       </c>
-      <c r="E42" s="195">
+      <c r="E42" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F42" s="195"/>
-      <c r="G42" s="196"/>
+      <c r="F42" s="194"/>
+      <c r="G42" s="195"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="191" t="s">
+      <c r="A43" s="190" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="192">
-        <v>0</v>
-      </c>
-      <c r="C43" s="192">
-        <v>0</v>
-      </c>
-      <c r="D43" s="192">
+      <c r="B43" s="191">
+        <v>0</v>
+      </c>
+      <c r="C43" s="191">
+        <v>0</v>
+      </c>
+      <c r="D43" s="191">
         <v>15</v>
       </c>
-      <c r="E43" s="192">
+      <c r="E43" s="191">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F43" s="192"/>
-      <c r="G43" s="193"/>
+      <c r="F43" s="191"/>
+      <c r="G43" s="192"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="194" t="s">
+      <c r="A44" s="193" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="195">
-        <v>0</v>
-      </c>
-      <c r="C44" s="195">
-        <v>0</v>
-      </c>
-      <c r="D44" s="195">
+      <c r="B44" s="194">
+        <v>0</v>
+      </c>
+      <c r="C44" s="194">
+        <v>0</v>
+      </c>
+      <c r="D44" s="194">
         <v>15</v>
       </c>
-      <c r="E44" s="195">
+      <c r="E44" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F44" s="195"/>
-      <c r="G44" s="196"/>
+      <c r="F44" s="194"/>
+      <c r="G44" s="195"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="191" t="s">
+      <c r="A45" s="190" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="192">
-        <v>0</v>
-      </c>
-      <c r="C45" s="192">
-        <v>0</v>
-      </c>
-      <c r="D45" s="192">
+      <c r="B45" s="191">
+        <v>0</v>
+      </c>
+      <c r="C45" s="191">
+        <v>0</v>
+      </c>
+      <c r="D45" s="191">
         <v>10</v>
       </c>
-      <c r="E45" s="192">
+      <c r="E45" s="191">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F45" s="192"/>
-      <c r="G45" s="193"/>
+      <c r="F45" s="191"/>
+      <c r="G45" s="192"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="194" t="s">
+      <c r="A46" s="193" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="195">
-        <v>0</v>
-      </c>
-      <c r="C46" s="195">
-        <v>0</v>
-      </c>
-      <c r="D46" s="195">
+      <c r="B46" s="194">
+        <v>0</v>
+      </c>
+      <c r="C46" s="194">
+        <v>0</v>
+      </c>
+      <c r="D46" s="194">
         <v>8</v>
       </c>
-      <c r="E46" s="195">
+      <c r="E46" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F46" s="195"/>
-      <c r="G46" s="196"/>
+      <c r="F46" s="194"/>
+      <c r="G46" s="195"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="191" t="s">
+      <c r="A47" s="190" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="192">
-        <v>0</v>
-      </c>
-      <c r="C47" s="192">
-        <v>0</v>
-      </c>
-      <c r="D47" s="192">
+      <c r="B47" s="191">
+        <v>0</v>
+      </c>
+      <c r="C47" s="191">
+        <v>0</v>
+      </c>
+      <c r="D47" s="191">
         <v>8</v>
       </c>
-      <c r="E47" s="192">
+      <c r="E47" s="191">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F47" s="192"/>
-      <c r="G47" s="193"/>
+      <c r="F47" s="191"/>
+      <c r="G47" s="192"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="194" t="s">
+      <c r="A48" s="193" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="195">
-        <v>0</v>
-      </c>
-      <c r="C48" s="195">
-        <v>0</v>
-      </c>
-      <c r="D48" s="195">
+      <c r="B48" s="194">
+        <v>0</v>
+      </c>
+      <c r="C48" s="194">
+        <v>0</v>
+      </c>
+      <c r="D48" s="194">
         <v>8</v>
       </c>
-      <c r="E48" s="195">
+      <c r="E48" s="194">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F48" s="195"/>
-      <c r="G48" s="196"/>
+      <c r="F48" s="194"/>
+      <c r="G48" s="195"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="197" t="s">
+      <c r="A49" s="196" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="198">
-        <v>0</v>
-      </c>
-      <c r="C49" s="198">
-        <v>0</v>
-      </c>
-      <c r="D49" s="198">
+      <c r="B49" s="197">
+        <v>0</v>
+      </c>
+      <c r="C49" s="197">
+        <v>0</v>
+      </c>
+      <c r="D49" s="197">
         <v>4</v>
       </c>
-      <c r="E49" s="198">
+      <c r="E49" s="197">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F49" s="198"/>
-      <c r="G49" s="199"/>
+      <c r="F49" s="197"/>
+      <c r="G49" s="198"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="200" t="s">
+      <c r="A50" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="201"/>
-      <c r="C50" s="201"/>
-      <c r="D50" s="201">
+      <c r="B50" s="200"/>
+      <c r="C50" s="200"/>
+      <c r="D50" s="200">
         <f>SUM(D41:D49)</f>
         <v>100</v>
       </c>
-      <c r="E50" s="202">
+      <c r="E50" s="201">
         <f>(SUM(E41:E49) +E52+E53+E54)/D50</f>
         <v>0</v>
       </c>
-      <c r="F50" s="202"/>
-      <c r="G50" s="203"/>
+      <c r="F50" s="201"/>
+      <c r="G50" s="202"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="204" t="s">
+      <c r="A51" s="203" t="s">
         <v>38</v>
       </c>
-      <c r="B51" s="205" t="s">
+      <c r="B51" s="204" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="205"/>
-      <c r="D51" s="205" t="s">
+      <c r="C51" s="204"/>
+      <c r="D51" s="204" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="206" t="s">
+      <c r="E51" s="205" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="206"/>
-      <c r="G51" s="207" t="s">
+      <c r="F51" s="205"/>
+      <c r="G51" s="206" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="208" t="s">
+      <c r="A52" s="207" t="s">
         <v>39</v>
       </c>
-      <c r="B52" s="209">
-        <v>0</v>
-      </c>
-      <c r="C52" s="209"/>
-      <c r="D52" s="210">
+      <c r="B52" s="208">
+        <v>0</v>
+      </c>
+      <c r="C52" s="208"/>
+      <c r="D52" s="209">
         <v>-10</v>
       </c>
-      <c r="E52" s="209">
+      <c r="E52" s="208">
         <f>B52*D52</f>
         <v>0</v>
       </c>
-      <c r="F52" s="209"/>
-      <c r="G52" s="211"/>
+      <c r="F52" s="208"/>
+      <c r="G52" s="210"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="212" t="s">
+      <c r="A53" s="211" t="s">
         <v>72</v>
       </c>
-      <c r="B53" s="213">
-        <v>0</v>
-      </c>
-      <c r="C53" s="213"/>
-      <c r="D53" s="214">
+      <c r="B53" s="212">
+        <v>0</v>
+      </c>
+      <c r="C53" s="212"/>
+      <c r="D53" s="213">
         <v>-15</v>
       </c>
-      <c r="E53" s="213">
+      <c r="E53" s="212">
         <f>B53*D53</f>
         <v>0</v>
       </c>
-      <c r="F53" s="213"/>
-      <c r="G53" s="215"/>
+      <c r="F53" s="212"/>
+      <c r="G53" s="214"/>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="216" t="s">
+      <c r="A54" s="215" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="217">
-        <v>0</v>
-      </c>
-      <c r="C54" s="217"/>
-      <c r="D54" s="218">
+      <c r="B54" s="216">
+        <v>0</v>
+      </c>
+      <c r="C54" s="216"/>
+      <c r="D54" s="217">
         <v>-5</v>
       </c>
-      <c r="E54" s="217">
+      <c r="E54" s="216">
         <f>B54*D54</f>
         <v>0</v>
       </c>
-      <c r="F54" s="217"/>
-      <c r="G54" s="219"/>
+      <c r="F54" s="216"/>
+      <c r="G54" s="218"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4117,8 +4117,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:Q60"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4138,85 +4138,85 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A2" s="240" t="s">
+      <c r="A2" s="239" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="240"/>
-      <c r="C2" s="240"/>
-      <c r="D2" s="240"/>
-      <c r="E2" s="240"/>
-      <c r="F2" s="240"/>
-      <c r="G2" s="240"/>
-      <c r="H2" s="240"/>
-      <c r="I2" s="240"/>
-      <c r="J2" s="240"/>
-      <c r="K2" s="240"/>
+      <c r="B2" s="239"/>
+      <c r="C2" s="239"/>
+      <c r="D2" s="239"/>
+      <c r="E2" s="239"/>
+      <c r="F2" s="239"/>
+      <c r="G2" s="239"/>
+      <c r="H2" s="239"/>
+      <c r="I2" s="239"/>
+      <c r="J2" s="239"/>
+      <c r="K2" s="239"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
     <row r="4" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A4" s="241" t="s">
+      <c r="A4" s="240" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="241"/>
-      <c r="C4" s="241"/>
-      <c r="D4" s="241"/>
-      <c r="E4" s="241"/>
-      <c r="F4" s="241"/>
-      <c r="G4" s="241"/>
-      <c r="H4" s="241"/>
-      <c r="I4" s="241"/>
-      <c r="J4" s="241"/>
-      <c r="K4" s="241"/>
+      <c r="B4" s="240"/>
+      <c r="C4" s="240"/>
+      <c r="D4" s="240"/>
+      <c r="E4" s="240"/>
+      <c r="F4" s="240"/>
+      <c r="G4" s="240"/>
+      <c r="H4" s="240"/>
+      <c r="I4" s="240"/>
+      <c r="J4" s="240"/>
+      <c r="K4" s="240"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:17" ht="18.75">
       <c r="A5" s="11"/>
-      <c r="B5" s="42"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="42"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="42"/>
+      <c r="H5" s="41"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="42"/>
+      <c r="K5" s="41"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A6" s="258" t="s">
+      <c r="A6" s="257" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="245" t="s">
+      <c r="B6" s="244" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="260" t="s">
+      <c r="C6" s="259" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="261"/>
-      <c r="E6" s="261"/>
-      <c r="F6" s="262" t="s">
+      <c r="D6" s="260"/>
+      <c r="E6" s="260"/>
+      <c r="F6" s="261" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="263"/>
-      <c r="H6" s="264"/>
-      <c r="I6" s="242" t="s">
+      <c r="G6" s="262"/>
+      <c r="H6" s="263"/>
+      <c r="I6" s="241" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="243"/>
-      <c r="K6" s="244"/>
+      <c r="J6" s="242"/>
+      <c r="K6" s="243"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="256"/>
-      <c r="O6" s="257"/>
-      <c r="P6" s="257"/>
+      <c r="N6" s="255"/>
+      <c r="O6" s="256"/>
+      <c r="P6" s="256"/>
     </row>
     <row r="7" spans="1:17" ht="18.75">
-      <c r="A7" s="259"/>
-      <c r="B7" s="246"/>
+      <c r="A7" s="258"/>
+      <c r="B7" s="245"/>
       <c r="C7" s="14" t="s">
         <v>13</v>
       </c>
@@ -4246,41 +4246,41 @@
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
     </row>
     <row r="8" spans="1:17" ht="18.75">
-      <c r="A8" s="255" t="s">
+      <c r="A8" s="254" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="255"/>
-      <c r="C8" s="248" t="s">
+      <c r="B8" s="254"/>
+      <c r="C8" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="249"/>
-      <c r="E8" s="47" t="s">
+      <c r="D8" s="248"/>
+      <c r="E8" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="248" t="s">
+      <c r="F8" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="249"/>
-      <c r="H8" s="47" t="s">
+      <c r="G8" s="248"/>
+      <c r="H8" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="248" t="s">
+      <c r="I8" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="249"/>
-      <c r="K8" s="47"/>
+      <c r="J8" s="248"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
     </row>
     <row r="9" spans="1:17" ht="121.5">
       <c r="A9" s="29" t="s">
@@ -4289,33 +4289,33 @@
       <c r="B9" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="101">
-        <v>1</v>
-      </c>
-      <c r="D9" s="99">
+      <c r="C9" s="100">
+        <v>1</v>
+      </c>
+      <c r="D9" s="98">
         <v>6</v>
       </c>
-      <c r="E9" s="102"/>
-      <c r="F9" s="103">
+      <c r="E9" s="101"/>
+      <c r="F9" s="102">
         <v>0.7</v>
       </c>
-      <c r="G9" s="100">
+      <c r="G9" s="99">
         <v>6</v>
       </c>
-      <c r="H9" s="104" t="s">
+      <c r="H9" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="105"/>
-      <c r="J9" s="106">
+      <c r="I9" s="104"/>
+      <c r="J9" s="105">
         <v>6</v>
       </c>
-      <c r="K9" s="107"/>
+      <c r="K9" s="106"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
     </row>
     <row r="10" spans="1:17" ht="45.75">
       <c r="A10" s="23" t="s">
@@ -4324,105 +4324,105 @@
       <c r="B10" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="101">
+      <c r="C10" s="100">
         <v>0.75</v>
       </c>
-      <c r="D10" s="99">
+      <c r="D10" s="98">
         <v>2</v>
       </c>
-      <c r="E10" s="102" t="s">
+      <c r="E10" s="101" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="103">
-        <v>1</v>
-      </c>
-      <c r="G10" s="100">
+      <c r="F10" s="102">
+        <v>1</v>
+      </c>
+      <c r="G10" s="99">
         <v>2</v>
       </c>
-      <c r="H10" s="104" t="s">
+      <c r="H10" s="103" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="105"/>
-      <c r="J10" s="106">
+      <c r="I10" s="104"/>
+      <c r="J10" s="105">
         <v>2</v>
       </c>
-      <c r="K10" s="107"/>
+      <c r="K10" s="106"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
     </row>
     <row r="11" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A11" s="250" t="s">
+      <c r="A11" s="249" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="251"/>
-      <c r="C11" s="48">
+      <c r="B11" s="250"/>
+      <c r="C11" s="47">
         <f>SUMPRODUCT(C6:C10,D6:D10)</f>
         <v>7.5</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="48">
         <f>SUM(D6:D10)</f>
         <v>8</v>
       </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="51">
+      <c r="E11" s="49"/>
+      <c r="F11" s="50">
         <f>SUMPRODUCT(F6:F10,G6:G10)</f>
         <v>6.1999999999999993</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="51">
         <f>SUM(G6:G10)</f>
         <v>8</v>
       </c>
-      <c r="H11" s="53"/>
-      <c r="I11" s="54">
+      <c r="H11" s="52"/>
+      <c r="I11" s="53">
         <f>SUMPRODUCT(I6:I10,J6:J10)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="55">
+      <c r="J11" s="54">
         <f>SUM(J6:J10)</f>
         <v>8</v>
       </c>
-      <c r="K11" s="56"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
     </row>
     <row r="12" spans="1:17" s="12" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A12" s="255" t="s">
+      <c r="A12" s="254" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="255"/>
-      <c r="C12" s="248" t="s">
+      <c r="B12" s="254"/>
+      <c r="C12" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="249"/>
-      <c r="E12" s="47" t="s">
+      <c r="D12" s="248"/>
+      <c r="E12" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="248" t="s">
+      <c r="F12" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="249"/>
-      <c r="H12" s="47" t="s">
+      <c r="G12" s="248"/>
+      <c r="H12" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="248" t="s">
+      <c r="I12" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="249"/>
-      <c r="K12" s="47"/>
+      <c r="J12" s="248"/>
+      <c r="K12" s="46"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
     </row>
     <row r="13" spans="1:17" ht="100.5" customHeight="1">
       <c r="A13" s="29" t="s">
@@ -4431,29 +4431,29 @@
       <c r="B13" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="80">
+      <c r="C13" s="79">
         <v>0.75</v>
       </c>
-      <c r="D13" s="81">
+      <c r="D13" s="80">
         <v>4</v>
       </c>
-      <c r="E13" s="82" t="s">
+      <c r="E13" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="90">
+      <c r="F13" s="89">
         <v>0.75</v>
       </c>
-      <c r="G13" s="91">
+      <c r="G13" s="90">
         <v>4</v>
       </c>
-      <c r="H13" s="92" t="s">
+      <c r="H13" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="I13" s="93"/>
-      <c r="J13" s="94">
+      <c r="I13" s="92"/>
+      <c r="J13" s="93">
         <v>4</v>
       </c>
-      <c r="K13" s="95"/>
+      <c r="K13" s="94"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
@@ -4464,27 +4464,27 @@
       <c r="B14" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="84">
-        <v>1</v>
-      </c>
-      <c r="D14" s="85">
+      <c r="C14" s="83">
+        <v>1</v>
+      </c>
+      <c r="D14" s="84">
         <v>2</v>
       </c>
-      <c r="E14" s="86"/>
-      <c r="F14" s="87">
-        <v>1</v>
-      </c>
-      <c r="G14" s="88">
+      <c r="E14" s="85"/>
+      <c r="F14" s="86">
+        <v>1</v>
+      </c>
+      <c r="G14" s="87">
         <v>2</v>
       </c>
-      <c r="H14" s="89" t="s">
+      <c r="H14" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="I14" s="77"/>
-      <c r="J14" s="78">
+      <c r="I14" s="76"/>
+      <c r="J14" s="77">
         <v>2</v>
       </c>
-      <c r="K14" s="79"/>
+      <c r="K14" s="78"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
@@ -4495,27 +4495,27 @@
       <c r="B15" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="84">
-        <v>1</v>
-      </c>
-      <c r="D15" s="85">
+      <c r="C15" s="83">
+        <v>1</v>
+      </c>
+      <c r="D15" s="84">
         <v>3</v>
       </c>
-      <c r="E15" s="86"/>
-      <c r="F15" s="87">
-        <v>1</v>
-      </c>
-      <c r="G15" s="88">
+      <c r="E15" s="85"/>
+      <c r="F15" s="86">
+        <v>1</v>
+      </c>
+      <c r="G15" s="87">
         <v>3</v>
       </c>
-      <c r="H15" s="89" t="s">
+      <c r="H15" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="I15" s="77"/>
-      <c r="J15" s="78">
+      <c r="I15" s="76"/>
+      <c r="J15" s="77">
         <v>3</v>
       </c>
-      <c r="K15" s="79"/>
+      <c r="K15" s="78"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
@@ -4526,27 +4526,27 @@
       <c r="B16" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="84">
-        <v>1</v>
-      </c>
-      <c r="D16" s="85">
+      <c r="C16" s="83">
+        <v>1</v>
+      </c>
+      <c r="D16" s="84">
         <v>2</v>
       </c>
-      <c r="E16" s="86"/>
-      <c r="F16" s="87">
-        <v>1</v>
-      </c>
-      <c r="G16" s="88">
+      <c r="E16" s="85"/>
+      <c r="F16" s="86">
+        <v>1</v>
+      </c>
+      <c r="G16" s="87">
         <v>2</v>
       </c>
-      <c r="H16" s="89" t="s">
+      <c r="H16" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="I16" s="77"/>
-      <c r="J16" s="78">
+      <c r="I16" s="76"/>
+      <c r="J16" s="77">
         <v>2</v>
       </c>
-      <c r="K16" s="79"/>
+      <c r="K16" s="78"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
@@ -4557,95 +4557,95 @@
       <c r="B17" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="84">
+      <c r="C17" s="83">
         <v>0.75</v>
       </c>
-      <c r="D17" s="85">
+      <c r="D17" s="84">
         <v>4</v>
       </c>
-      <c r="E17" s="86" t="s">
+      <c r="E17" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="87">
-        <v>0</v>
-      </c>
-      <c r="G17" s="88">
+      <c r="F17" s="86">
+        <v>0</v>
+      </c>
+      <c r="G17" s="87">
         <v>4</v>
       </c>
-      <c r="H17" s="89" t="s">
+      <c r="H17" s="88" t="s">
         <v>100</v>
       </c>
-      <c r="I17" s="77"/>
-      <c r="J17" s="78">
+      <c r="I17" s="76"/>
+      <c r="J17" s="77">
         <v>4</v>
       </c>
-      <c r="K17" s="79"/>
+      <c r="K17" s="78"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A18" s="250" t="s">
+      <c r="A18" s="249" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="251"/>
-      <c r="C18" s="48">
+      <c r="B18" s="250"/>
+      <c r="C18" s="47">
         <f>SUMPRODUCT(C13:C17,D13:D17)</f>
         <v>13</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="48">
         <f>SUM(D13:D17)</f>
         <v>15</v>
       </c>
-      <c r="E18" s="50"/>
-      <c r="F18" s="51">
+      <c r="E18" s="49"/>
+      <c r="F18" s="50">
         <f>SUMPRODUCT(F13:F17,G13:G17)</f>
         <v>10</v>
       </c>
-      <c r="G18" s="52">
+      <c r="G18" s="51">
         <f>SUM(G13:G17)</f>
         <v>15</v>
       </c>
-      <c r="H18" s="53"/>
-      <c r="I18" s="54">
+      <c r="H18" s="52"/>
+      <c r="I18" s="53">
         <f>SUMPRODUCT(I13:I17,J13:J17)</f>
         <v>0</v>
       </c>
-      <c r="J18" s="55">
+      <c r="J18" s="54">
         <f>SUM(J13:J17)</f>
         <v>15</v>
       </c>
-      <c r="K18" s="56"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-    </row>
-    <row r="19" spans="1:17" s="44" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A19" s="247" t="s">
+      <c r="K18" s="55"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44"/>
+      <c r="Q18" s="44"/>
+    </row>
+    <row r="19" spans="1:17" s="43" customFormat="1" ht="18.399999999999999" customHeight="1">
+      <c r="A19" s="246" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="247"/>
-      <c r="C19" s="248" t="s">
+      <c r="B19" s="246"/>
+      <c r="C19" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="249"/>
-      <c r="E19" s="47" t="s">
+      <c r="D19" s="248"/>
+      <c r="E19" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="248" t="s">
+      <c r="F19" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="249"/>
-      <c r="H19" s="47" t="s">
+      <c r="G19" s="248"/>
+      <c r="H19" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="248" t="s">
+      <c r="I19" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="249"/>
-      <c r="K19" s="47"/>
+      <c r="J19" s="248"/>
+      <c r="K19" s="46"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
@@ -4656,14 +4656,14 @@
       <c r="B20" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="98">
+      <c r="C20" s="97">
         <v>1</v>
       </c>
       <c r="D20" s="25">
         <v>2</v>
       </c>
       <c r="E20" s="26"/>
-      <c r="F20" s="83">
+      <c r="F20" s="82">
         <v>0.5</v>
       </c>
       <c r="G20" s="27">
@@ -4672,11 +4672,11 @@
       <c r="H20" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="I20" s="74"/>
-      <c r="J20" s="75">
+      <c r="I20" s="73"/>
+      <c r="J20" s="74">
         <v>2</v>
       </c>
-      <c r="K20" s="76"/>
+      <c r="K20" s="75"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
@@ -4687,27 +4687,27 @@
       <c r="B21" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="84">
-        <v>1</v>
-      </c>
-      <c r="D21" s="85">
+      <c r="C21" s="83">
+        <v>1</v>
+      </c>
+      <c r="D21" s="84">
         <v>3</v>
       </c>
-      <c r="E21" s="86"/>
-      <c r="F21" s="87">
-        <v>1</v>
-      </c>
-      <c r="G21" s="88">
+      <c r="E21" s="85"/>
+      <c r="F21" s="86">
+        <v>1</v>
+      </c>
+      <c r="G21" s="87">
         <v>3</v>
       </c>
-      <c r="H21" s="89" t="s">
+      <c r="H21" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="I21" s="77"/>
-      <c r="J21" s="78">
+      <c r="I21" s="76"/>
+      <c r="J21" s="77">
         <v>3</v>
       </c>
-      <c r="K21" s="79"/>
+      <c r="K21" s="78"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
@@ -4718,109 +4718,109 @@
       <c r="B22" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="84">
+      <c r="C22" s="83">
         <v>0.9</v>
       </c>
-      <c r="D22" s="85">
+      <c r="D22" s="84">
         <v>3</v>
       </c>
-      <c r="E22" s="86" t="s">
+      <c r="E22" s="85" t="s">
         <v>109</v>
       </c>
-      <c r="F22" s="87">
-        <v>1</v>
-      </c>
-      <c r="G22" s="88">
+      <c r="F22" s="86">
+        <v>1</v>
+      </c>
+      <c r="G22" s="87">
         <v>3</v>
       </c>
-      <c r="H22" s="89" t="s">
+      <c r="H22" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="77"/>
-      <c r="J22" s="78">
+      <c r="I22" s="76"/>
+      <c r="J22" s="77">
         <v>3</v>
       </c>
-      <c r="K22" s="79"/>
+      <c r="K22" s="78"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:17" s="45" customFormat="1" ht="15.75">
-      <c r="A23" s="252" t="s">
+    <row r="23" spans="1:17" s="44" customFormat="1" ht="15.75">
+      <c r="A23" s="251" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="253"/>
-      <c r="C23" s="58">
+      <c r="B23" s="252"/>
+      <c r="C23" s="57">
         <f>SUMPRODUCT(C20:C22,D20:D22)</f>
         <v>7.7</v>
       </c>
-      <c r="D23" s="59">
+      <c r="D23" s="58">
         <f>SUM(D20:D22)</f>
         <v>8</v>
       </c>
-      <c r="E23" s="60"/>
-      <c r="F23" s="61">
+      <c r="E23" s="59"/>
+      <c r="F23" s="60">
         <f>SUMPRODUCT(F20:F22,G20:G22)</f>
         <v>7</v>
       </c>
-      <c r="G23" s="62">
+      <c r="G23" s="61">
         <f>SUM(G20:G22)</f>
         <v>8</v>
       </c>
-      <c r="H23" s="63"/>
-      <c r="I23" s="64">
+      <c r="H23" s="62"/>
+      <c r="I23" s="63">
         <f>SUMPRODUCT(I20:I22,J20:J22)</f>
         <v>0</v>
       </c>
-      <c r="J23" s="65">
+      <c r="J23" s="64">
         <f>SUM(J20:J22)</f>
         <v>8</v>
       </c>
-      <c r="K23" s="66"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
     </row>
     <row r="24" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="B24" s="46"/>
-      <c r="C24" s="248" t="s">
+      <c r="B24" s="45"/>
+      <c r="C24" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="249"/>
-      <c r="E24" s="47" t="s">
+      <c r="D24" s="248"/>
+      <c r="E24" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="248" t="s">
+      <c r="F24" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="249"/>
-      <c r="H24" s="47" t="s">
+      <c r="G24" s="248"/>
+      <c r="H24" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="248" t="s">
+      <c r="I24" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="J24" s="249"/>
-      <c r="K24" s="47"/>
+      <c r="J24" s="248"/>
+      <c r="K24" s="46"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:17" ht="76.5">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="98">
+      <c r="C25" s="97">
         <v>1</v>
       </c>
       <c r="D25" s="25">
         <v>2</v>
       </c>
       <c r="E25" s="26"/>
-      <c r="F25" s="83">
+      <c r="F25" s="82">
         <v>0.5</v>
       </c>
       <c r="G25" s="27">
@@ -4829,11 +4829,11 @@
       <c r="H25" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="I25" s="74"/>
-      <c r="J25" s="75">
+      <c r="I25" s="73"/>
+      <c r="J25" s="74">
         <v>2</v>
       </c>
-      <c r="K25" s="76"/>
+      <c r="K25" s="75"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
     </row>
@@ -4844,25 +4844,25 @@
       <c r="B26" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="84">
-        <v>1</v>
-      </c>
-      <c r="D26" s="85">
-        <v>1</v>
-      </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="87">
-        <v>1</v>
-      </c>
-      <c r="G26" s="88">
-        <v>1</v>
-      </c>
-      <c r="H26" s="89"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="78">
-        <v>1</v>
-      </c>
-      <c r="K26" s="79"/>
+      <c r="C26" s="83">
+        <v>1</v>
+      </c>
+      <c r="D26" s="84">
+        <v>1</v>
+      </c>
+      <c r="E26" s="85"/>
+      <c r="F26" s="86">
+        <v>1</v>
+      </c>
+      <c r="G26" s="87">
+        <v>1</v>
+      </c>
+      <c r="H26" s="88"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="77">
+        <v>1</v>
+      </c>
+      <c r="K26" s="78"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
     </row>
@@ -4873,85 +4873,85 @@
       <c r="B27" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="84">
-        <v>1</v>
-      </c>
-      <c r="D27" s="85">
-        <v>1</v>
-      </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="87">
+      <c r="C27" s="83">
+        <v>1</v>
+      </c>
+      <c r="D27" s="84">
+        <v>1</v>
+      </c>
+      <c r="E27" s="85"/>
+      <c r="F27" s="86">
         <v>0.5</v>
       </c>
-      <c r="G27" s="88">
-        <v>1</v>
-      </c>
-      <c r="H27" s="89" t="s">
+      <c r="G27" s="87">
+        <v>1</v>
+      </c>
+      <c r="H27" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="I27" s="77"/>
-      <c r="J27" s="78">
-        <v>1</v>
-      </c>
-      <c r="K27" s="79"/>
+      <c r="I27" s="76"/>
+      <c r="J27" s="77">
+        <v>1</v>
+      </c>
+      <c r="K27" s="78"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
     </row>
-    <row r="28" spans="1:17" s="45" customFormat="1" ht="15.75">
-      <c r="A28" s="254" t="s">
+    <row r="28" spans="1:17" s="44" customFormat="1" ht="15.75">
+      <c r="A28" s="253" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="253"/>
-      <c r="C28" s="48">
+      <c r="B28" s="252"/>
+      <c r="C28" s="47">
         <f>SUMPRODUCT(C25:C27,D25:D27)</f>
         <v>4</v>
       </c>
-      <c r="D28" s="49">
+      <c r="D28" s="48">
         <f>SUM(D25:D27)</f>
         <v>4</v>
       </c>
-      <c r="E28" s="50"/>
-      <c r="F28" s="61">
+      <c r="E28" s="49"/>
+      <c r="F28" s="60">
         <f>SUMPRODUCT(F25:F27,G25:G27)</f>
         <v>2.5</v>
       </c>
-      <c r="G28" s="62">
+      <c r="G28" s="61">
         <f>SUM(G25:G27)</f>
         <v>4</v>
       </c>
-      <c r="H28" s="63"/>
-      <c r="I28" s="64">
+      <c r="H28" s="62"/>
+      <c r="I28" s="63">
         <f>SUMPRODUCT(I25:I27,J25:J27)</f>
         <v>0</v>
       </c>
-      <c r="J28" s="65">
+      <c r="J28" s="64">
         <f>SUM(J25:J27)</f>
         <v>4</v>
       </c>
-      <c r="K28" s="66"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
     </row>
     <row r="29" spans="1:17" ht="21" customHeight="1">
-      <c r="A29" s="247" t="s">
+      <c r="A29" s="246" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="247"/>
-      <c r="C29" s="248" t="s">
+      <c r="B29" s="246"/>
+      <c r="C29" s="247" t="s">
         <v>120</v>
       </c>
-      <c r="D29" s="249"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="248" t="s">
+      <c r="D29" s="248"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="247" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="249"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="248" t="s">
+      <c r="G29" s="248"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="J29" s="249"/>
-      <c r="K29" s="47"/>
+      <c r="J29" s="248"/>
+      <c r="K29" s="46"/>
       <c r="L29" s="9"/>
       <c r="M29" s="4"/>
     </row>
@@ -4962,27 +4962,27 @@
       <c r="B30" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="C30" s="80">
+      <c r="C30" s="79">
         <v>0.2</v>
       </c>
-      <c r="D30" s="81">
+      <c r="D30" s="80">
         <v>2</v>
       </c>
-      <c r="E30" s="82" t="s">
+      <c r="E30" s="81" t="s">
         <v>123</v>
       </c>
-      <c r="F30" s="90">
-        <v>1</v>
-      </c>
-      <c r="G30" s="91">
+      <c r="F30" s="89">
+        <v>1</v>
+      </c>
+      <c r="G30" s="90">
         <v>2</v>
       </c>
-      <c r="H30" s="96"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="94">
+      <c r="H30" s="95"/>
+      <c r="I30" s="92"/>
+      <c r="J30" s="93">
         <v>2</v>
       </c>
-      <c r="K30" s="95"/>
+      <c r="K30" s="94"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
     </row>
@@ -4993,25 +4993,25 @@
       <c r="B31" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="84">
-        <v>1</v>
-      </c>
-      <c r="D31" s="85">
+      <c r="C31" s="83">
+        <v>1</v>
+      </c>
+      <c r="D31" s="84">
         <v>2</v>
       </c>
-      <c r="E31" s="86"/>
-      <c r="F31" s="87">
-        <v>1</v>
-      </c>
-      <c r="G31" s="88">
+      <c r="E31" s="85"/>
+      <c r="F31" s="86">
+        <v>1</v>
+      </c>
+      <c r="G31" s="87">
         <v>2</v>
       </c>
-      <c r="H31" s="97"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="78">
+      <c r="H31" s="96"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="77">
         <v>2</v>
       </c>
-      <c r="K31" s="79"/>
+      <c r="K31" s="78"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
     </row>
@@ -5022,29 +5022,29 @@
       <c r="B32" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="84">
+      <c r="C32" s="83">
         <v>0.2</v>
       </c>
-      <c r="D32" s="85">
+      <c r="D32" s="84">
         <v>2</v>
       </c>
-      <c r="E32" s="86" t="s">
+      <c r="E32" s="85" t="s">
         <v>128</v>
       </c>
-      <c r="F32" s="87">
-        <v>0</v>
-      </c>
-      <c r="G32" s="88">
+      <c r="F32" s="86">
+        <v>0</v>
+      </c>
+      <c r="G32" s="87">
         <v>2</v>
       </c>
-      <c r="H32" s="97" t="s">
+      <c r="H32" s="96" t="s">
         <v>129</v>
       </c>
-      <c r="I32" s="77"/>
-      <c r="J32" s="78">
+      <c r="I32" s="76"/>
+      <c r="J32" s="77">
         <v>2</v>
       </c>
-      <c r="K32" s="79"/>
+      <c r="K32" s="78"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
     </row>
@@ -5055,91 +5055,91 @@
       <c r="B33" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="84">
+      <c r="C33" s="83">
         <v>0.4</v>
       </c>
-      <c r="D33" s="85">
+      <c r="D33" s="84">
         <v>3</v>
       </c>
-      <c r="E33" s="86" t="s">
+      <c r="E33" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="F33" s="87">
+      <c r="F33" s="86">
         <v>0.5</v>
       </c>
-      <c r="G33" s="88">
+      <c r="G33" s="87">
         <v>3</v>
       </c>
-      <c r="H33" s="97" t="s">
+      <c r="H33" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="I33" s="77"/>
-      <c r="J33" s="78">
+      <c r="I33" s="76"/>
+      <c r="J33" s="77">
         <v>3</v>
       </c>
-      <c r="K33" s="79"/>
+      <c r="K33" s="78"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
     </row>
-    <row r="34" spans="1:13" s="45" customFormat="1" ht="32.25">
-      <c r="A34" s="250" t="s">
+    <row r="34" spans="1:13" s="44" customFormat="1" ht="32.25">
+      <c r="A34" s="249" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="251"/>
-      <c r="C34" s="48">
+      <c r="B34" s="250"/>
+      <c r="C34" s="47">
         <f>SUMPRODUCT(C30:C33,D30:D33)</f>
         <v>4</v>
       </c>
-      <c r="D34" s="49">
+      <c r="D34" s="48">
         <f>SUM(D30:D33)</f>
         <v>9</v>
       </c>
-      <c r="E34" s="50" t="s">
+      <c r="E34" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="F34" s="51">
+      <c r="F34" s="50">
         <f>SUMPRODUCT(F30:F33,G30:G33)</f>
         <v>5.5</v>
       </c>
-      <c r="G34" s="52">
+      <c r="G34" s="51">
         <f>SUM(G30:G33)</f>
         <v>9</v>
       </c>
-      <c r="H34" s="68" t="s">
+      <c r="H34" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="I34" s="64">
+      <c r="I34" s="63">
         <f>SUMPRODUCT(I30:I33,J30:J33)</f>
         <v>0</v>
       </c>
-      <c r="J34" s="65">
+      <c r="J34" s="64">
         <f>SUM(J30:J33)</f>
         <v>9</v>
       </c>
-      <c r="K34" s="66"/>
-      <c r="L34" s="57"/>
-      <c r="M34" s="57"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="56"/>
+      <c r="M34" s="56"/>
     </row>
     <row r="35" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A35" s="255" t="s">
+      <c r="A35" s="254" t="s">
         <v>136</v>
       </c>
-      <c r="B35" s="255"/>
-      <c r="C35" s="248" t="s">
+      <c r="B35" s="254"/>
+      <c r="C35" s="247" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="249"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="248" t="s">
+      <c r="D35" s="248"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="247" t="s">
         <v>120</v>
       </c>
-      <c r="G35" s="249"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="69" t="s">
+      <c r="G35" s="248"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="J35" s="67"/>
-      <c r="K35" s="47"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="46"/>
       <c r="L35" s="8"/>
       <c r="M35" s="4"/>
     </row>
@@ -5150,29 +5150,29 @@
       <c r="B36" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="C36" s="80">
-        <v>0</v>
-      </c>
-      <c r="D36" s="81">
+      <c r="C36" s="79">
+        <v>0</v>
+      </c>
+      <c r="D36" s="80">
         <v>2</v>
       </c>
-      <c r="E36" s="82" t="s">
+      <c r="E36" s="81" t="s">
         <v>139</v>
       </c>
-      <c r="F36" s="90">
-        <v>0</v>
-      </c>
-      <c r="G36" s="91">
+      <c r="F36" s="89">
+        <v>0</v>
+      </c>
+      <c r="G36" s="90">
         <v>2</v>
       </c>
-      <c r="H36" s="92" t="s">
+      <c r="H36" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="I36" s="93"/>
-      <c r="J36" s="94">
+      <c r="I36" s="92"/>
+      <c r="J36" s="93">
         <v>2</v>
       </c>
-      <c r="K36" s="95"/>
+      <c r="K36" s="94"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
     </row>
@@ -5183,29 +5183,29 @@
       <c r="B37" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="C37" s="84">
+      <c r="C37" s="83">
         <v>0.65</v>
       </c>
-      <c r="D37" s="85">
+      <c r="D37" s="84">
         <v>2</v>
       </c>
-      <c r="E37" s="86" t="s">
+      <c r="E37" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="F37" s="87">
-        <v>1</v>
-      </c>
-      <c r="G37" s="88">
+      <c r="F37" s="86">
+        <v>1</v>
+      </c>
+      <c r="G37" s="87">
         <v>2</v>
       </c>
-      <c r="H37" s="89" t="s">
+      <c r="H37" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="I37" s="77"/>
-      <c r="J37" s="78">
+      <c r="I37" s="76"/>
+      <c r="J37" s="77">
         <v>2</v>
       </c>
-      <c r="K37" s="79"/>
+      <c r="K37" s="78"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
     </row>
@@ -5216,27 +5216,27 @@
       <c r="B38" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="84">
-        <v>1</v>
-      </c>
-      <c r="D38" s="85">
+      <c r="C38" s="83">
+        <v>1</v>
+      </c>
+      <c r="D38" s="84">
         <v>3</v>
       </c>
-      <c r="E38" s="86"/>
-      <c r="F38" s="87">
+      <c r="E38" s="85"/>
+      <c r="F38" s="86">
         <v>0.5</v>
       </c>
-      <c r="G38" s="88">
+      <c r="G38" s="87">
         <v>3</v>
       </c>
-      <c r="H38" s="89" t="s">
+      <c r="H38" s="88" t="s">
         <v>146</v>
       </c>
-      <c r="I38" s="77"/>
-      <c r="J38" s="78">
+      <c r="I38" s="76"/>
+      <c r="J38" s="77">
         <v>3</v>
       </c>
-      <c r="K38" s="79"/>
+      <c r="K38" s="78"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
     </row>
@@ -5247,95 +5247,95 @@
       <c r="B39" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="C39" s="84">
-        <v>0</v>
-      </c>
-      <c r="D39" s="85">
+      <c r="C39" s="83">
+        <v>0</v>
+      </c>
+      <c r="D39" s="84">
         <v>3</v>
       </c>
-      <c r="E39" s="86" t="s">
+      <c r="E39" s="85" t="s">
         <v>149</v>
       </c>
-      <c r="F39" s="87">
+      <c r="F39" s="86">
         <v>0.5</v>
       </c>
-      <c r="G39" s="88">
+      <c r="G39" s="87">
         <v>3</v>
       </c>
-      <c r="H39" s="89" t="s">
+      <c r="H39" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="I39" s="77"/>
-      <c r="J39" s="78">
+      <c r="I39" s="76"/>
+      <c r="J39" s="77">
         <v>3</v>
       </c>
-      <c r="K39" s="79"/>
+      <c r="K39" s="78"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
     </row>
-    <row r="40" spans="1:13" s="45" customFormat="1" ht="48.75">
-      <c r="A40" s="250" t="s">
+    <row r="40" spans="1:13" s="44" customFormat="1" ht="48.75">
+      <c r="A40" s="249" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="251"/>
-      <c r="C40" s="70">
+      <c r="B40" s="250"/>
+      <c r="C40" s="69">
         <f>SUMPRODUCT(C36:C39,D36:D39)</f>
         <v>4.3</v>
       </c>
-      <c r="D40" s="49">
+      <c r="D40" s="48">
         <f>SUM(D36:D39)</f>
         <v>10</v>
       </c>
-      <c r="E40" s="50" t="s">
+      <c r="E40" s="49" t="s">
         <v>151</v>
       </c>
-      <c r="F40" s="71">
+      <c r="F40" s="70">
         <f>SUMPRODUCT(F36:F39,G36:G39)</f>
         <v>5</v>
       </c>
-      <c r="G40" s="52">
+      <c r="G40" s="51">
         <f>SUM(G36:G39)</f>
         <v>10</v>
       </c>
-      <c r="H40" s="53" t="s">
+      <c r="H40" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="I40" s="64">
+      <c r="I40" s="63">
         <f>SUMPRODUCT(I36:I39,J36:J39)</f>
         <v>0</v>
       </c>
-      <c r="J40" s="65">
+      <c r="J40" s="64">
         <f>SUM(J36:J39)</f>
         <v>10</v>
       </c>
-      <c r="K40" s="66"/>
-      <c r="L40" s="57"/>
-      <c r="M40" s="57"/>
+      <c r="K40" s="65"/>
+      <c r="L40" s="56"/>
+      <c r="M40" s="56"/>
     </row>
     <row r="41" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="248" t="s">
+      <c r="B41" s="45"/>
+      <c r="C41" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="249"/>
-      <c r="E41" s="67" t="s">
+      <c r="D41" s="248"/>
+      <c r="E41" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="248" t="s">
+      <c r="F41" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="249"/>
-      <c r="H41" s="47" t="s">
+      <c r="G41" s="248"/>
+      <c r="H41" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="I41" s="248" t="s">
+      <c r="I41" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="J41" s="249"/>
-      <c r="K41" s="47"/>
+      <c r="J41" s="248"/>
+      <c r="K41" s="46"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
     </row>
@@ -5346,29 +5346,29 @@
       <c r="B42" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="84">
+      <c r="C42" s="83">
         <v>0.5</v>
       </c>
-      <c r="D42" s="85">
+      <c r="D42" s="84">
         <v>2</v>
       </c>
-      <c r="E42" s="86" t="s">
+      <c r="E42" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="F42" s="87">
-        <v>1</v>
-      </c>
-      <c r="G42" s="88">
+      <c r="F42" s="86">
+        <v>1</v>
+      </c>
+      <c r="G42" s="87">
         <v>2</v>
       </c>
-      <c r="H42" s="89" t="s">
+      <c r="H42" s="88" t="s">
         <v>157</v>
       </c>
-      <c r="I42" s="77"/>
-      <c r="J42" s="78">
+      <c r="I42" s="76"/>
+      <c r="J42" s="77">
         <v>2</v>
       </c>
-      <c r="K42" s="79"/>
+      <c r="K42" s="78"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
     </row>
@@ -5379,29 +5379,29 @@
       <c r="B43" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="C43" s="84">
+      <c r="C43" s="83">
         <v>0.5</v>
       </c>
-      <c r="D43" s="85">
+      <c r="D43" s="84">
         <v>2</v>
       </c>
-      <c r="E43" s="86" t="s">
+      <c r="E43" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="F43" s="87">
+      <c r="F43" s="86">
         <v>0.75</v>
       </c>
-      <c r="G43" s="88">
+      <c r="G43" s="87">
         <v>2</v>
       </c>
-      <c r="H43" s="89" t="s">
+      <c r="H43" s="88" t="s">
         <v>161</v>
       </c>
-      <c r="I43" s="77"/>
-      <c r="J43" s="78">
+      <c r="I43" s="76"/>
+      <c r="J43" s="77">
         <v>2</v>
       </c>
-      <c r="K43" s="79"/>
+      <c r="K43" s="78"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
     </row>
@@ -5412,25 +5412,25 @@
       <c r="B44" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="C44" s="84">
-        <v>1</v>
-      </c>
-      <c r="D44" s="85">
+      <c r="C44" s="83">
+        <v>1</v>
+      </c>
+      <c r="D44" s="84">
         <v>2</v>
       </c>
-      <c r="E44" s="86"/>
-      <c r="F44" s="87">
-        <v>1</v>
-      </c>
-      <c r="G44" s="88">
+      <c r="E44" s="85"/>
+      <c r="F44" s="86">
+        <v>1</v>
+      </c>
+      <c r="G44" s="87">
         <v>2</v>
       </c>
-      <c r="H44" s="89"/>
-      <c r="I44" s="77"/>
-      <c r="J44" s="78">
+      <c r="H44" s="88"/>
+      <c r="I44" s="76"/>
+      <c r="J44" s="77">
         <v>2</v>
       </c>
-      <c r="K44" s="79"/>
+      <c r="K44" s="78"/>
       <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:13" ht="152.25">
@@ -5440,30 +5440,30 @@
       <c r="B45" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="84">
+      <c r="C45" s="83">
         <f>1.5/4</f>
         <v>0.375</v>
       </c>
-      <c r="D45" s="85">
+      <c r="D45" s="84">
         <v>4</v>
       </c>
-      <c r="E45" s="86" t="s">
+      <c r="E45" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="F45" s="87">
-        <v>1</v>
-      </c>
-      <c r="G45" s="88">
+      <c r="F45" s="86">
+        <v>1</v>
+      </c>
+      <c r="G45" s="87">
         <v>4</v>
       </c>
-      <c r="H45" s="89" t="s">
+      <c r="H45" s="88" t="s">
         <v>167</v>
       </c>
-      <c r="I45" s="77"/>
-      <c r="J45" s="78">
+      <c r="I45" s="76"/>
+      <c r="J45" s="77">
         <v>4</v>
       </c>
-      <c r="K45" s="79"/>
+      <c r="K45" s="78"/>
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
     </row>
@@ -5474,30 +5474,30 @@
       <c r="B46" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="C46" s="84">
+      <c r="C46" s="83">
         <v>0.75</v>
       </c>
-      <c r="D46" s="85">
+      <c r="D46" s="84">
         <v>6</v>
       </c>
-      <c r="E46" s="86" t="s">
+      <c r="E46" s="85" t="s">
         <v>170</v>
       </c>
-      <c r="F46" s="87">
+      <c r="F46" s="86">
         <f>4/6</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G46" s="88">
+      <c r="G46" s="87">
         <v>6</v>
       </c>
-      <c r="H46" s="89" t="s">
+      <c r="H46" s="88" t="s">
         <v>171</v>
       </c>
-      <c r="I46" s="77"/>
-      <c r="J46" s="78">
+      <c r="I46" s="76"/>
+      <c r="J46" s="77">
         <v>6</v>
       </c>
-      <c r="K46" s="79"/>
+      <c r="K46" s="78"/>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
     </row>
@@ -5508,29 +5508,29 @@
       <c r="B47" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="C47" s="84">
+      <c r="C47" s="83">
         <v>0.9</v>
       </c>
-      <c r="D47" s="85">
+      <c r="D47" s="84">
         <v>10</v>
       </c>
-      <c r="E47" s="86" t="s">
+      <c r="E47" s="85" t="s">
         <v>174</v>
       </c>
-      <c r="F47" s="87">
-        <v>1</v>
-      </c>
-      <c r="G47" s="88">
+      <c r="F47" s="86">
+        <v>1</v>
+      </c>
+      <c r="G47" s="87">
         <v>10</v>
       </c>
-      <c r="H47" s="89" t="s">
+      <c r="H47" s="88" t="s">
         <v>175</v>
       </c>
-      <c r="I47" s="77"/>
-      <c r="J47" s="78">
+      <c r="I47" s="76"/>
+      <c r="J47" s="77">
         <v>10</v>
       </c>
-      <c r="K47" s="79"/>
+      <c r="K47" s="78"/>
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
     </row>
@@ -5541,31 +5541,31 @@
       <c r="B48" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="C48" s="84">
+      <c r="C48" s="83">
         <f>3/6</f>
         <v>0.5</v>
       </c>
-      <c r="D48" s="85">
+      <c r="D48" s="84">
         <v>6</v>
       </c>
-      <c r="E48" s="86" t="s">
+      <c r="E48" s="85" t="s">
         <v>178</v>
       </c>
-      <c r="F48" s="87">
+      <c r="F48" s="86">
         <f>4/6</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G48" s="88">
+      <c r="G48" s="87">
         <v>6</v>
       </c>
-      <c r="H48" s="89" t="s">
+      <c r="H48" s="88" t="s">
         <v>179</v>
       </c>
-      <c r="I48" s="77"/>
-      <c r="J48" s="78">
+      <c r="I48" s="76"/>
+      <c r="J48" s="77">
         <v>6</v>
       </c>
-      <c r="K48" s="79"/>
+      <c r="K48" s="78"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
     </row>
@@ -5576,91 +5576,91 @@
       <c r="B49" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="C49" s="84">
-        <v>1</v>
-      </c>
-      <c r="D49" s="85">
+      <c r="C49" s="83">
+        <v>1</v>
+      </c>
+      <c r="D49" s="84">
         <v>3</v>
       </c>
-      <c r="E49" s="86"/>
-      <c r="F49" s="87">
-        <v>1</v>
-      </c>
-      <c r="G49" s="88">
+      <c r="E49" s="85"/>
+      <c r="F49" s="86">
+        <v>1</v>
+      </c>
+      <c r="G49" s="87">
         <v>3</v>
       </c>
-      <c r="H49" s="89"/>
-      <c r="I49" s="77"/>
-      <c r="J49" s="78">
+      <c r="H49" s="88"/>
+      <c r="I49" s="76"/>
+      <c r="J49" s="77">
         <v>3</v>
       </c>
-      <c r="K49" s="79"/>
+      <c r="K49" s="78"/>
       <c r="L49" s="5"/>
       <c r="M49" s="5"/>
     </row>
     <row r="50" spans="1:17" s="30" customFormat="1" ht="48.75">
-      <c r="A50" s="250" t="s">
+      <c r="A50" s="249" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="251"/>
-      <c r="C50" s="72">
+      <c r="B50" s="250"/>
+      <c r="C50" s="71">
         <f>SUMPRODUCT(C42:C49,D42:D49)</f>
         <v>25</v>
       </c>
-      <c r="D50" s="59">
+      <c r="D50" s="58">
         <f>SUM(D42:D49)</f>
         <v>35</v>
       </c>
-      <c r="E50" s="60" t="s">
+      <c r="E50" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="F50" s="71">
+      <c r="F50" s="70">
         <f>SUMPRODUCT(F42:F49,G42:G49)</f>
         <v>30.5</v>
       </c>
-      <c r="G50" s="52">
+      <c r="G50" s="51">
         <f>SUM(G42:G49)</f>
         <v>35</v>
       </c>
-      <c r="H50" s="53" t="s">
+      <c r="H50" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="I50" s="54">
+      <c r="I50" s="53">
         <f>SUMPRODUCT(I42:I49,J42:J49)</f>
         <v>0</v>
       </c>
-      <c r="J50" s="55">
+      <c r="J50" s="54">
         <f>SUM(J42:J49)</f>
         <v>35</v>
       </c>
-      <c r="K50" s="56"/>
-      <c r="L50" s="57"/>
-      <c r="M50" s="57"/>
-      <c r="N50" s="45"/>
-      <c r="O50" s="45"/>
-      <c r="P50" s="45"/>
-      <c r="Q50" s="45"/>
+      <c r="K50" s="55"/>
+      <c r="L50" s="56"/>
+      <c r="M50" s="56"/>
+      <c r="N50" s="44"/>
+      <c r="O50" s="44"/>
+      <c r="P50" s="44"/>
+      <c r="Q50" s="44"/>
     </row>
     <row r="51" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A51" s="255" t="s">
+      <c r="A51" s="254" t="s">
         <v>184</v>
       </c>
-      <c r="B51" s="255"/>
-      <c r="C51" s="248" t="s">
+      <c r="B51" s="254"/>
+      <c r="C51" s="247" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="249"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="248" t="s">
+      <c r="D51" s="248"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="247" t="s">
         <v>120</v>
       </c>
-      <c r="G51" s="249"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="248" t="s">
+      <c r="G51" s="248"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="247" t="s">
         <v>16</v>
       </c>
-      <c r="J51" s="249"/>
-      <c r="K51" s="47"/>
+      <c r="J51" s="248"/>
+      <c r="K51" s="46"/>
       <c r="L51" s="8"/>
       <c r="M51" s="4"/>
     </row>
@@ -5671,25 +5671,25 @@
       <c r="B52" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="C52" s="80">
-        <v>1</v>
-      </c>
-      <c r="D52" s="81">
+      <c r="C52" s="79">
+        <v>1</v>
+      </c>
+      <c r="D52" s="80">
         <v>2</v>
       </c>
-      <c r="E52" s="82"/>
-      <c r="F52" s="83">
+      <c r="E52" s="81"/>
+      <c r="F52" s="82">
         <v>1</v>
       </c>
       <c r="G52" s="27">
         <v>2</v>
       </c>
       <c r="H52" s="28"/>
-      <c r="I52" s="74"/>
-      <c r="J52" s="75">
+      <c r="I52" s="73"/>
+      <c r="J52" s="74">
         <v>2</v>
       </c>
-      <c r="K52" s="76"/>
+      <c r="K52" s="75"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
     </row>
@@ -5700,29 +5700,29 @@
       <c r="B53" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="C53" s="84">
+      <c r="C53" s="83">
         <v>0.25</v>
       </c>
-      <c r="D53" s="85">
+      <c r="D53" s="84">
         <v>2</v>
       </c>
-      <c r="E53" s="86" t="s">
+      <c r="E53" s="85" t="s">
         <v>189</v>
       </c>
-      <c r="F53" s="87">
-        <v>0</v>
-      </c>
-      <c r="G53" s="88">
+      <c r="F53" s="86">
+        <v>0</v>
+      </c>
+      <c r="G53" s="87">
         <v>2</v>
       </c>
-      <c r="H53" s="223" t="s">
+      <c r="H53" s="222" t="s">
         <v>190</v>
       </c>
-      <c r="I53" s="77"/>
-      <c r="J53" s="78">
+      <c r="I53" s="76"/>
+      <c r="J53" s="77">
         <v>2</v>
       </c>
-      <c r="K53" s="79"/>
+      <c r="K53" s="78"/>
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
     </row>
@@ -5733,25 +5733,25 @@
       <c r="B54" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="C54" s="84">
-        <v>1</v>
-      </c>
-      <c r="D54" s="85">
-        <v>1</v>
-      </c>
-      <c r="E54" s="86"/>
-      <c r="F54" s="87">
-        <v>1</v>
-      </c>
-      <c r="G54" s="88">
-        <v>1</v>
-      </c>
-      <c r="H54" s="89"/>
-      <c r="I54" s="77"/>
-      <c r="J54" s="78">
-        <v>1</v>
-      </c>
-      <c r="K54" s="79"/>
+      <c r="C54" s="83">
+        <v>1</v>
+      </c>
+      <c r="D54" s="84">
+        <v>1</v>
+      </c>
+      <c r="E54" s="85"/>
+      <c r="F54" s="86">
+        <v>1</v>
+      </c>
+      <c r="G54" s="87">
+        <v>1</v>
+      </c>
+      <c r="H54" s="88"/>
+      <c r="I54" s="76"/>
+      <c r="J54" s="77">
+        <v>1</v>
+      </c>
+      <c r="K54" s="78"/>
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
     </row>
@@ -5762,31 +5762,31 @@
       <c r="B55" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="C55" s="84">
+      <c r="C55" s="83">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D55" s="85">
+      <c r="D55" s="84">
         <v>4</v>
       </c>
-      <c r="E55" s="86" t="s">
+      <c r="E55" s="85" t="s">
         <v>195</v>
       </c>
-      <c r="F55" s="87">
+      <c r="F55" s="86">
         <f>0.5</f>
         <v>0.5</v>
       </c>
-      <c r="G55" s="88">
+      <c r="G55" s="87">
         <v>4</v>
       </c>
-      <c r="H55" s="89" t="s">
+      <c r="H55" s="88" t="s">
         <v>196</v>
       </c>
-      <c r="I55" s="77"/>
-      <c r="J55" s="78">
+      <c r="I55" s="76"/>
+      <c r="J55" s="77">
         <v>4</v>
       </c>
-      <c r="K55" s="79"/>
+      <c r="K55" s="78"/>
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
     </row>
@@ -5797,91 +5797,91 @@
       <c r="B56" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="C56" s="84">
+      <c r="C56" s="83">
         <v>0.9</v>
       </c>
-      <c r="D56" s="85">
+      <c r="D56" s="84">
         <v>2</v>
       </c>
-      <c r="E56" s="86" t="s">
+      <c r="E56" s="85" t="s">
         <v>199</v>
       </c>
-      <c r="F56" s="87">
-        <v>1</v>
-      </c>
-      <c r="G56" s="88">
+      <c r="F56" s="86">
+        <v>1</v>
+      </c>
+      <c r="G56" s="87">
         <v>2</v>
       </c>
-      <c r="H56" s="89"/>
-      <c r="I56" s="77"/>
-      <c r="J56" s="78">
+      <c r="H56" s="88"/>
+      <c r="I56" s="76"/>
+      <c r="J56" s="77">
         <v>2</v>
       </c>
-      <c r="K56" s="79"/>
+      <c r="K56" s="78"/>
       <c r="L56" s="6"/>
       <c r="M56" s="5"/>
     </row>
-    <row r="57" spans="1:17" s="45" customFormat="1" ht="129">
-      <c r="A57" s="250" t="s">
+    <row r="57" spans="1:17" s="44" customFormat="1" ht="129">
+      <c r="A57" s="249" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="251"/>
-      <c r="C57" s="58">
+      <c r="B57" s="250"/>
+      <c r="C57" s="57">
         <f>SUMPRODUCT(C52:C56,D52:D56)</f>
         <v>7.9666666666666659</v>
       </c>
-      <c r="D57" s="59">
+      <c r="D57" s="58">
         <f>SUM(D52:D56)</f>
         <v>11</v>
       </c>
-      <c r="E57" s="60" t="s">
+      <c r="E57" s="59" t="s">
         <v>200</v>
       </c>
-      <c r="F57" s="61">
+      <c r="F57" s="60">
         <f>SUMPRODUCT(F52:F56,G52:G56)</f>
         <v>7</v>
       </c>
-      <c r="G57" s="62">
+      <c r="G57" s="61">
         <f>SUM(G52:G56)</f>
         <v>11</v>
       </c>
-      <c r="H57" s="63" t="s">
+      <c r="H57" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="I57" s="54">
+      <c r="I57" s="53">
         <f>SUMPRODUCT(I52:I56,J52:J56)</f>
         <v>0</v>
       </c>
-      <c r="J57" s="55">
+      <c r="J57" s="54">
         <f>SUM(J52:J56)</f>
         <v>11</v>
       </c>
-      <c r="K57" s="56"/>
-      <c r="L57" s="57"/>
-      <c r="M57" s="57"/>
+      <c r="K57" s="55"/>
+      <c r="L57" s="56"/>
+      <c r="M57" s="56"/>
     </row>
     <row r="58" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A58" s="278" t="s">
+      <c r="A58" s="277" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="279"/>
-      <c r="C58" s="279"/>
-      <c r="D58" s="279"/>
-      <c r="E58" s="279"/>
-      <c r="F58" s="279"/>
-      <c r="G58" s="279"/>
-      <c r="H58" s="279"/>
-      <c r="I58" s="279"/>
-      <c r="J58" s="279"/>
-      <c r="K58" s="280"/>
+      <c r="B58" s="278"/>
+      <c r="C58" s="278"/>
+      <c r="D58" s="278"/>
+      <c r="E58" s="278"/>
+      <c r="F58" s="278"/>
+      <c r="G58" s="278"/>
+      <c r="H58" s="278"/>
+      <c r="I58" s="278"/>
+      <c r="J58" s="278"/>
+      <c r="K58" s="279"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
     </row>
     <row r="59" spans="1:17">
-      <c r="A59" s="265" t="s">
+      <c r="A59" s="264" t="s">
         <v>202</v>
       </c>
-      <c r="B59" s="266"/>
+      <c r="B59" s="265"/>
       <c r="C59" s="34">
         <f>C11+C18+C23+C28+C34+C40+C50+C57</f>
         <v>73.466666666666669</v>
@@ -5891,16 +5891,16 @@
         <v>100</v>
       </c>
       <c r="E59" s="26"/>
-      <c r="F59" s="35">
-        <f>F18+F23+F28+F34+F40+F50+F57</f>
-        <v>67.5</v>
+      <c r="F59" s="280">
+        <f>F11+F18+F23+F28+F34+F50+F57</f>
+        <v>68.7</v>
       </c>
       <c r="G59" s="27">
         <f>G11+G18+G23+G28+G34+G40+G50+G57</f>
         <v>100</v>
       </c>
       <c r="H59" s="28"/>
-      <c r="I59" s="36">
+      <c r="I59" s="35">
         <f>I18+I23+I28+I34+I40+I50+I57</f>
         <v>0</v>
       </c>
@@ -5912,31 +5912,31 @@
       <c r="L59" s="6"/>
       <c r="M59" s="5"/>
     </row>
-    <row r="60" spans="1:17" s="45" customFormat="1" ht="15.75">
-      <c r="A60" s="267" t="s">
+    <row r="60" spans="1:17" s="44" customFormat="1" ht="15.75">
+      <c r="A60" s="266" t="s">
         <v>203</v>
       </c>
-      <c r="B60" s="268"/>
-      <c r="C60" s="269">
+      <c r="B60" s="267"/>
+      <c r="C60" s="268">
         <f>C59/D59</f>
         <v>0.73466666666666669</v>
       </c>
-      <c r="D60" s="270"/>
-      <c r="E60" s="271"/>
-      <c r="F60" s="272">
+      <c r="D60" s="269"/>
+      <c r="E60" s="270"/>
+      <c r="F60" s="271">
         <f>F59/G59</f>
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="G60" s="273"/>
-      <c r="H60" s="274"/>
-      <c r="I60" s="275">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="G60" s="272"/>
+      <c r="H60" s="273"/>
+      <c r="I60" s="274">
         <f>I59/J59</f>
         <v>0</v>
       </c>
-      <c r="J60" s="276"/>
-      <c r="K60" s="277"/>
-      <c r="L60" s="73"/>
-      <c r="M60" s="73"/>
+      <c r="J60" s="275"/>
+      <c r="K60" s="276"/>
+      <c r="L60" s="72"/>
+      <c r="M60" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="51">

</xml_diff>